<commit_message>
fully working - link missing
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,16 @@
           <t>00_Slide</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0_Comment</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>0_Replies</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -451,11 +461,155 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test2.pptx</t>
+          <t>eventdrivenarchitecture.pptx</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>test 1 slide 1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Is there an examples of what this "envelope" could look like?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes, it is a cloud event, which I've now referenced</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>We should consider defining this word "hydrated" somewhere.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>I've reworded, but I will use the word "re-hydrate" in the CQRS slide</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[@Mott, Chad] Should you mention that idempotency supports at-least-once delivery?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>I'm not sure I follow... idempotent services are _resiliant_ to at least once, which I explain in the headline</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Is the purpose to have test events in lower environments?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>17</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Could be more specific than "as things happen".</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>I've reworded this</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>eventdrivenarchitecture.pptx</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Why are these items lettered and the previous items numbered?</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>I see what you are saying... I've added a heading above A and B to hopefully clarify (they are numbered b/c there are 3 of them, whereas the letters correspond to letters on the left</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>